<commit_message>
2.20 test map update
</commit_message>
<xml_diff>
--- a/src/maps/test.xlsx
+++ b/src/maps/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DKU\CompSci\201\Campus\src\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B6177E-8ABC-463E-8FBC-10769EA94A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3C052E-28B7-4FD1-BAB4-C73F09E579F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,15 +353,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -371,8 +371,14 @@
       <c r="C1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -386,7 +392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -400,7 +406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -414,7 +420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -428,7 +434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>

</xml_diff>